<commit_message>
[kibot] Executed Kibot script to generate documentation, manufacturing and assembly data
</commit_message>
<xml_diff>
--- a/kibot/bom/generic_bom.xlsx
+++ b/kibot/bom/generic_bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
   <si>
     <t>Row</t>
   </si>
@@ -47,6 +47,21 @@
     <t>Datasheet</t>
   </si>
   <si>
+    <t>qr_version</t>
+  </si>
+  <si>
+    <t>qr_size</t>
+  </si>
+  <si>
+    <t>qr_ecc</t>
+  </si>
+  <si>
+    <t>qr_mask</t>
+  </si>
+  <si>
+    <t>qr_text</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -59,6 +74,9 @@
     <t>LD1 LD3</t>
   </si>
   <si>
+    <t>APA102</t>
+  </si>
+  <si>
     <t>APA102-Strip-Output</t>
   </si>
   <si>
@@ -71,6 +89,9 @@
     <t>~</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>LD2</t>
   </si>
   <si>
@@ -89,6 +110,9 @@
     <t>X4.1 X4.2</t>
   </si>
   <si>
+    <t>Cable-0.7mm</t>
+  </si>
+  <si>
     <t>Solder-Pad-THT-0.7mm</t>
   </si>
   <si>
@@ -98,12 +122,33 @@
     <t>X5.1 X5.2</t>
   </si>
   <si>
+    <t>Cable-1.5mm</t>
+  </si>
+  <si>
     <t>Solder-Pad-THT-1.5mm</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>4-pin DIN connector</t>
+  </si>
+  <si>
+    <t>DIN-4</t>
+  </si>
+  <si>
+    <t>X1 X2</t>
+  </si>
+  <si>
+    <t>KLB-4</t>
+  </si>
+  <si>
+    <t>Lumberg-KLB-4-Klinkensteckverbinder-3_5-180deg-turnable</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -116,22 +161,13 @@
     <t>XT30</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>X1 X2</t>
-  </si>
-  <si>
-    <t>Lumberg-KLB-4-Klinkensteckverbinder-3_5-180deg-turnable</t>
-  </si>
-  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
     <t>Schematic:</t>
   </si>
   <si>
-    <t>LightPipe_Out_PCB</t>
+    <t>LightPipe_PCB</t>
   </si>
   <si>
     <t>Variant:</t>
@@ -149,13 +185,13 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2020-02-10</t>
+    <t>2023-04-07</t>
   </si>
   <si>
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.10-86aedd382b~118~ubuntu20.04.1</t>
+    <t>6.0.11-2627ca5db0~126~ubuntu20.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -682,7 +718,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -700,11 +736,16 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1">
+    <row r="1" spans="1:14" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -712,78 +753,83 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:14">
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:14">
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F6" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -811,184 +857,289 @@
       <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1">
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="H10" s="9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1">
+        <v>22</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="I11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="J11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="I12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="H13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="I13" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1009,22 +1160,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Kibot] Run job 'basic-export' and '3d-export'
</commit_message>
<xml_diff>
--- a/kibot/bom/generic_bom.xlsx
+++ b/kibot/bom/generic_bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
   <si>
     <t>Row</t>
   </si>
@@ -47,6 +47,21 @@
     <t>Datasheet</t>
   </si>
   <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>MFN</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>MF1</t>
+  </si>
+  <si>
+    <t>MFN1</t>
+  </si>
+  <si>
     <t>qr_version</t>
   </si>
   <si>
@@ -131,19 +146,34 @@
     <t>5</t>
   </si>
   <si>
-    <t>4-pin DIN connector</t>
-  </si>
-  <si>
-    <t>DIN-4</t>
+    <t>Audio Jack, 4 Poles (TRRS)</t>
+  </si>
+  <si>
+    <t>AudioJack4</t>
   </si>
   <si>
     <t>X1 X2</t>
   </si>
   <si>
-    <t>KLB-4</t>
-  </si>
-  <si>
-    <t>Lumberg-KLB-4-Klinkensteckverbinder-3_5-180deg-turnable</t>
+    <t>Lumberg KLB4</t>
+  </si>
+  <si>
+    <t>Lumberg-KLB-4-Jack-3_5-180deg-turnable</t>
+  </si>
+  <si>
+    <t>https://downloads.lumberg.com/datenblaetter/en/klb4.pdf</t>
+  </si>
+  <si>
+    <t>Lumberg</t>
+  </si>
+  <si>
+    <t>KLB4</t>
+  </si>
+  <si>
+    <t>HUXUAN</t>
+  </si>
+  <si>
+    <t>PJ392</t>
   </si>
   <si>
     <t>6</t>
@@ -161,6 +191,18 @@
     <t>XT30</t>
   </si>
   <si>
+    <t>https://datasheet.lcsc.com/lcsc/2207151430_Changzhou-Amass-Elec-XT30UPB30-F-G--_C108769.pdf</t>
+  </si>
+  <si>
+    <t>Changzhou Amass Elec</t>
+  </si>
+  <si>
+    <t>XT30UPB30-F.G.*</t>
+  </si>
+  <si>
+    <t>C108769</t>
+  </si>
+  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
@@ -179,7 +221,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>v0.1.0</t>
+    <t>v0.1.1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -718,7 +760,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -732,20 +774,25 @@
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="60.7109375" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32" customHeight="1">
+    <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -758,78 +805,83 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="F6" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -872,274 +924,379 @@
       <c r="N8" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1">
+      <c r="O8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="H10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="I11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="J11" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="30" customHeight="1">
       <c r="A12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>22</v>
-      </c>
       <c r="J12" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>28</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="C1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1160,22 +1317,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try to run KiBot - but it does not work well with KiCad 7.0 → Downgrade to KiCad 6.0?
</commit_message>
<xml_diff>
--- a/kibot/bom/generic_bom.xlsx
+++ b/kibot/bom/generic_bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>Row</t>
   </si>
@@ -53,7 +53,7 @@
     <t>MFN</t>
   </si>
   <si>
-    <t>LCSC</t>
+    <t>LCSC#</t>
   </si>
   <si>
     <t>MF1</t>
@@ -80,19 +80,19 @@
     <t>1</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x04, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_01x04</t>
-  </si>
-  <si>
-    <t>LD1 LD3</t>
-  </si>
-  <si>
-    <t>APA102</t>
-  </si>
-  <si>
-    <t>APA102-Strip-Output</t>
+    <t>Audio Jack, 4 Poles (TRRS)</t>
+  </si>
+  <si>
+    <t>AudioJack4</t>
+  </si>
+  <si>
+    <t>X1 X2</t>
+  </si>
+  <si>
+    <t>Lumberg KLB4</t>
+  </si>
+  <si>
+    <t>Lumberg-KLB-4-Jack-3_5-180deg-turnable</t>
   </si>
   <si>
     <t>2</t>
@@ -101,84 +101,24 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>~</t>
+    <t>https://downloads.lumberg.com/datenblaetter/en/klb4.pdf</t>
+  </si>
+  <si>
+    <t>Lumberg</t>
+  </si>
+  <si>
+    <t>KLB4</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>LD2</t>
-  </si>
-  <si>
-    <t>APA102-Strip-Input</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x01, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_01x01</t>
-  </si>
-  <si>
-    <t>X4.1 X4.2</t>
-  </si>
-  <si>
-    <t>Cable-0.7mm</t>
-  </si>
-  <si>
-    <t>Solder-Pad-THT-0.7mm</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>X5.1 X5.2</t>
-  </si>
-  <si>
-    <t>Cable-1.5mm</t>
-  </si>
-  <si>
-    <t>Solder-Pad-THT-1.5mm</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Audio Jack, 4 Poles (TRRS)</t>
-  </si>
-  <si>
-    <t>AudioJack4</t>
-  </si>
-  <si>
-    <t>X1 X2</t>
-  </si>
-  <si>
-    <t>Lumberg KLB4</t>
-  </si>
-  <si>
-    <t>Lumberg-KLB-4-Jack-3_5-180deg-turnable</t>
-  </si>
-  <si>
-    <t>https://downloads.lumberg.com/datenblaetter/en/klb4.pdf</t>
-  </si>
-  <si>
-    <t>Lumberg</t>
-  </si>
-  <si>
-    <t>KLB4</t>
-  </si>
-  <si>
     <t>HUXUAN</t>
   </si>
   <si>
     <t>PJ392</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -233,7 +173,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.11-2627ca5db0~126~ubuntu20.04.1</t>
+    <t>7.0.8-7.0.8~ubuntu22.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -242,7 +182,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>10 (4 SMD/ 6 THT)</t>
+    <t>3 (0 SMD/ 3 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -760,7 +700,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -772,7 +712,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="43.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -780,7 +720,7 @@
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" customWidth="1"/>
@@ -792,7 +732,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -813,55 +753,55 @@
     </row>
     <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F2" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -869,16 +809,16 @@
     </row>
     <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="F6" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -940,7 +880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30" customHeight="1">
+    <row r="9" spans="1:19">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -965,38 +905,38 @@
       <c r="H9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>28</v>
+      <c r="K9" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="30" customHeight="1">
@@ -1004,19 +944,19 @@
         <v>25</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>19</v>
@@ -1024,274 +964,38 @@
       <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>28</v>
+      <c r="I10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="30" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="S12" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="S13" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="30" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="R14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="S14" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1317,22 +1021,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized KiBot script to make it work as good as possible with KiCad 7.0
</commit_message>
<xml_diff>
--- a/kibot/bom/generic_bom.xlsx
+++ b/kibot/bom/generic_bom.xlsx
@@ -161,13 +161,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>v0.1.1</t>
+    <t>v0.1.2</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-04-07</t>
+    <t>2023-10-26</t>
   </si>
   <si>
     <t>KiCad Version:</t>

</xml_diff>